<commit_message>
clean up main folder
</commit_message>
<xml_diff>
--- a/data/data_cleaning/Brumberg_BCCA_revisions_costa_recode.xlsx
+++ b/data/data_cleaning/Brumberg_BCCA_revisions_costa_recode.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\Documents\GitHub\BCCAch7\data\data_cleaning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/lade8828_colorado_edu/Documents/Documents/GitHub/BCCAch7/data/data_cleaning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F342F108-B481-4092-A700-0D65CDBAD9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F342F108-B481-4092-A700-0D65CDBAD9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D12D1390-EAE0-5543-81E3-B4621052693D}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{287F872C-E026-F34C-9B25-F2439A05DFA8}"/>
+    <workbookView xWindow="-5120" yWindow="1920" windowWidth="30240" windowHeight="17800" xr2:uid="{287F872C-E026-F34C-9B25-F2439A05DFA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -587,10 +587,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -613,17 +621,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -958,13 +969,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8183EE3-ECF6-A14B-85E7-F81342B03AA6}">
   <dimension ref="A1:ES3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BW3" workbookViewId="0">
-      <selection activeCell="CT4" sqref="CT4"/>
+    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:149" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1413,7 +1427,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:149" ht="408" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:149" ht="408" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>41</v>
       </c>
@@ -1426,7 +1440,7 @@
       <c r="D2" t="s">
         <v>153</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>154</v>
       </c>
       <c r="F2" t="s">
@@ -1691,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:149" ht="408" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:149" ht="408" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>41</v>
       </c>
@@ -1964,6 +1978,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{5D3231D3-A04D-834A-919D-2FFE7133BC03}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>